<commit_message>
Added new settings values:  - employee quarterly rates;  - names of functional groups;  - hourly production calendar;  - other.
</commit_message>
<xml_diff>
--- a/Parameters/FNSusbst.xlsx
+++ b/Parameters/FNSusbst.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB759A2-F85E-4A11-A504-322CC0D69A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62079B0-F807-4E72-A162-DABE47B51253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>ProjectNum</t>
   </si>
@@ -61,9 +61,6 @@
     <t>А0402 - Декретный отпуск (факт=плану)</t>
   </si>
   <si>
-    <t>&lt;нет ФН&gt;</t>
-  </si>
-  <si>
     <t>В0318 Организация работ подразделений ДРЭО</t>
   </si>
   <si>
@@ -101,6 +98,36 @@
   </si>
   <si>
     <t>СУП</t>
+  </si>
+  <si>
+    <t>(нет ФН)</t>
+  </si>
+  <si>
+    <t>Д0611 - КИС "Единая ГИС"</t>
+  </si>
+  <si>
+    <t>ГиД</t>
+  </si>
+  <si>
+    <t>А0602 - Адм. Время. RCBI. Отпуск</t>
+  </si>
+  <si>
+    <t>А0603 - Адм. Время. RCBI. Больничный</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>П0558 - Отраслевой шаблон ГиД на S/4HANA</t>
+  </si>
+  <si>
+    <t>ERP</t>
+  </si>
+  <si>
+    <t>Т0598 - Система учета трудозатрат ЛТ</t>
+  </si>
+  <si>
+    <t>КИС</t>
   </si>
 </sst>
 </file>
@@ -455,11 +482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,95 +556,135 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>